<commit_message>
Get current Login info
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Sem8\SWP391\2_SWP391\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BADDA535-DA59-4B15-806F-70CA0F9F84B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB63E53A-8755-45B2-9B79-21D269420194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12504" firstSheet="2" activeTab="4" xr2:uid="{E3278138-A7B9-4E4A-A15C-31336F4552C1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="3" xr2:uid="{E3278138-A7B9-4E4A-A15C-31336F4552C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Spiece" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="238">
   <si>
     <t>ID</t>
   </si>
@@ -62,9 +62,6 @@
     <t>phần trên màu nâu và phần dưới màu trắng với hai bên sườn bóng và một cái cựa sẫm màu chạy trên bầu ngực ngang vai. Nó có mào đen nhọn cao, mặt đỏ và đường viền đen mỏng. Đuôi dài và có màu nâu với các đầu lông màu trắng, nhưng vùng lỗ thông hơi có màu đỏ. Con non thiếu mảng đỏ phía sau mắt và vùng lỗ thông hơi có màu cam đỏ</t>
   </si>
   <si>
-    <t>420px-Red-whiskered_bulbul_by_Creepanta_11.jpg (420×630) (wikimedia.org)</t>
-  </si>
-  <si>
     <t>Chào mào</t>
   </si>
   <si>
@@ -89,9 +86,6 @@
     <t>https://youtu.be/oRHcP8lYaL0</t>
   </si>
   <si>
-    <t>image3-1632998835-30-width650height460.jpg (650×460) (eva.vn)</t>
-  </si>
-  <si>
     <t>Khi sống trong môi trường tự nhiên, chim Họa Mi thường kiếm ăn từ các lớp lá theo từng cặp hoặc bầy đàn. chim Họa Mi thường sinh sản vào tầm tháng 6 – 7 Âm lịch. Tổ của chim Họa Mi thường làm từ lá tre, cỏ và rễ cây. Vào mùa sinh sản chim Họa Mi thường đẻ từ 2 – 5 trứng và ấp trong vòng 13 – 16 ngày, sau đó chim bố, chim mẹ sẽ kiếm ăn nuôi con. </t>
   </si>
   <si>
@@ -110,9 +104,6 @@
     <t>https://youtu.be/88-LGgj1GBQ</t>
   </si>
   <si>
-    <t>x2qa9iwXtlPBwn3_s0Of700Z45jLsv3y_qHdrfsHTbEJbKGaQFlCIgMp7BsVeHNDY_t1Y3FZyTk44hwXnY9ZTymKEGOe8dMiBsEyM3X_jFZN11XQX2yw4OC_a8ef_8mlPk5jD0Gn (1200×627) (googleusercontent.com)</t>
-  </si>
-  <si>
     <t>Vành Khuyên</t>
   </si>
   <si>
@@ -125,9 +116,6 @@
     <t>Thích sống nơi có khí hậu ấm áp như Châu Phi, Nam Á, Úc và Đông Nam Á</t>
   </si>
   <si>
-    <t>image1-1633053449-421-width600height450.jpg (600×450) (eva.vn)</t>
-  </si>
-  <si>
     <t>https://youtu.be/vwYrsyHWEJM</t>
   </si>
   <si>
@@ -717,6 +705,48 @@
   </si>
   <si>
     <t>11/1/2023  10:00:00 AM</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/thumb/f/fa/Red-whiskered_bulbul_by_Creepanta_11.jpg/420px-Red-whiskered_bulbul_by_Creepanta_11.jpg</t>
+  </si>
+  <si>
+    <t>https://cdn.eva.vn/upload/3-2021/images/2021-09-30/image3-1632998835-30-width650height460.jpg</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/x2qa9iwXtlPBwn3_s0Of700Z45jLsv3y_qHdrfsHTbEJbKGaQFlCIgMp7BsVeHNDY_t1Y3FZyTk44hwXnY9ZTymKEGOe8dMiBsEyM3X_jFZN11XQX2yw4OC_a8ef_8mlPk5jD0Gn</t>
+  </si>
+  <si>
+    <t>https://cdn.eva.vn/upload/4-2021/images/2021-10-01/image1-1633053449-421-width600height450.jpg</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>birdid</t>
+  </si>
+  <si>
+    <t>cageid</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Detail</t>
+  </si>
+  <si>
+    <t>0011</t>
+  </si>
+  <si>
+    <t>Chuyển lồng</t>
+  </si>
+  <si>
+    <t>Chuyển lồng do thay lông</t>
+  </si>
+  <si>
+    <t>Chuyển lồng do bị thương</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chuyển lồng </t>
   </si>
 </sst>
 </file>
@@ -1142,7 +1172,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1176,7 +1206,7 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="H1" t="s">
         <v>6</v>
@@ -1187,118 +1217,118 @@
     </row>
     <row r="2" spans="1:9" ht="114.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>9</v>
+        <v>224</v>
       </c>
       <c r="G2">
         <v>11</v>
       </c>
       <c r="H2" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="144" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="105.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
       <c r="C3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="F3" s="3" t="s">
-        <v>18</v>
+        <v>225</v>
       </c>
       <c r="G3">
         <v>17</v>
       </c>
       <c r="H3" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="244.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="259.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="E4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="F4" s="3" t="s">
-        <v>25</v>
+        <v>226</v>
       </c>
       <c r="G4">
         <v>8</v>
       </c>
       <c r="H4" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="144" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="B5" t="s">
-        <v>26</v>
-      </c>
       <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="F5" s="3" t="s">
-        <v>30</v>
+        <v>227</v>
       </c>
       <c r="G5">
         <v>7</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" display="https://upload.wikimedia.org/wikipedia/commons/thumb/f/fa/Red-whiskered_bulbul_by_Creepanta_11.jpg/420px-Red-whiskered_bulbul_by_Creepanta_11.jpg" xr:uid="{017CAC94-250D-48ED-AE07-AB65B10789C7}"/>
-    <hyperlink ref="E2" r:id="rId2" tooltip="Chỉa sẻ liên kết" xr:uid="{E494B199-8B9A-4C00-83DF-18B90459E855}"/>
-    <hyperlink ref="E3" r:id="rId3" tooltip="Chỉa sẻ liên kết" xr:uid="{6D5AEA0E-73E3-4667-A286-5169A6E56BA3}"/>
-    <hyperlink ref="F3" r:id="rId4" display="https://cdn.eva.vn/upload/3-2021/images/2021-09-30/image3-1632998835-30-width650height460.jpg" xr:uid="{39410BA9-BFA4-4BA9-830C-4A5A0B07C901}"/>
-    <hyperlink ref="E4" r:id="rId5" tooltip="Chỉa sẻ liên kết" xr:uid="{0B9BC2BC-7167-421E-9B9D-3BF0155DE8D0}"/>
-    <hyperlink ref="F4" r:id="rId6" display="https://lh3.googleusercontent.com/x2qa9iwXtlPBwn3_s0Of700Z45jLsv3y_qHdrfsHTbEJbKGaQFlCIgMp7BsVeHNDY_t1Y3FZyTk44hwXnY9ZTymKEGOe8dMiBsEyM3X_jFZN11XQX2yw4OC_a8ef_8mlPk5jD0Gn" xr:uid="{E6818EFC-5754-4C39-8C0D-8414AFE88C14}"/>
-    <hyperlink ref="F5" r:id="rId7" display="https://cdn.eva.vn/upload/4-2021/images/2021-10-01/image1-1633053449-421-width600height450.jpg" xr:uid="{9D946949-687E-4AAC-928B-7DECAFD980B1}"/>
-    <hyperlink ref="E5" r:id="rId8" tooltip="Chỉa sẻ liên kết" xr:uid="{CAD03E34-E954-4634-A6F4-6B5BA57891AD}"/>
+    <hyperlink ref="E2" r:id="rId1" tooltip="Chỉa sẻ liên kết" xr:uid="{E494B199-8B9A-4C00-83DF-18B90459E855}"/>
+    <hyperlink ref="E3" r:id="rId2" tooltip="Chỉa sẻ liên kết" xr:uid="{6D5AEA0E-73E3-4667-A286-5169A6E56BA3}"/>
+    <hyperlink ref="F3" r:id="rId3" xr:uid="{39410BA9-BFA4-4BA9-830C-4A5A0B07C901}"/>
+    <hyperlink ref="E4" r:id="rId4" tooltip="Chỉa sẻ liên kết" xr:uid="{0B9BC2BC-7167-421E-9B9D-3BF0155DE8D0}"/>
+    <hyperlink ref="F5" r:id="rId5" xr:uid="{9D946949-687E-4AAC-928B-7DECAFD980B1}"/>
+    <hyperlink ref="E5" r:id="rId6" tooltip="Chỉa sẻ liên kết" xr:uid="{CAD03E34-E954-4634-A6F4-6B5BA57891AD}"/>
+    <hyperlink ref="F2" r:id="rId7" xr:uid="{CC16B704-B0FF-4190-9C9A-4D99B6947B03}"/>
+    <hyperlink ref="F4" r:id="rId8" xr:uid="{A5E4398E-8339-445E-97D7-DEAC1EC40911}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId9"/>
@@ -1309,8 +1339,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8636BF8E-BA53-4F84-A925-0B2EA1242A50}">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1326,498 +1356,498 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" t="s">
         <v>32</v>
       </c>
-      <c r="C1" t="s">
+      <c r="H1" t="s">
         <v>33</v>
       </c>
-      <c r="D1" t="s">
+      <c r="I1" t="s">
         <v>34</v>
       </c>
-      <c r="E1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F1" t="s">
-        <v>62</v>
-      </c>
-      <c r="G1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I1" t="s">
+    </row>
+    <row r="2" spans="1:9" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
-        <v>42</v>
       </c>
       <c r="B2" s="10">
         <v>44867</v>
       </c>
       <c r="C2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" t="s">
         <v>60</v>
       </c>
-      <c r="D2" t="s">
-        <v>64</v>
-      </c>
       <c r="E2" s="3" t="s">
-        <v>9</v>
+        <v>224</v>
       </c>
       <c r="F2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="H2" s="9" t="str">
         <f>Spiece!$A$2</f>
         <v>001</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B3" s="10">
         <v>44868</v>
       </c>
       <c r="C3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>9</v>
+        <v>224</v>
       </c>
       <c r="F3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="H3" s="9" t="str">
         <f>Spiece!$A$2</f>
         <v>001</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B4" s="10">
         <v>44869</v>
       </c>
       <c r="C4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>18</v>
+        <v>225</v>
       </c>
       <c r="F4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="H4" s="9" t="str">
         <f>Spiece!$A$3</f>
         <v>002</v>
       </c>
       <c r="I4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B5" s="10">
         <v>44870</v>
       </c>
       <c r="C5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>18</v>
+        <v>225</v>
       </c>
       <c r="F5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="H5" s="9" t="str">
         <f>Spiece!$A$3</f>
         <v>002</v>
       </c>
       <c r="I5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B6" s="10">
         <v>44871</v>
       </c>
       <c r="C6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>25</v>
+        <v>226</v>
       </c>
       <c r="F6" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="H6" s="9" t="str">
         <f>Spiece!$A$4</f>
         <v>003</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B7" s="10">
         <v>44872</v>
       </c>
       <c r="C7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>25</v>
+        <v>226</v>
       </c>
       <c r="F7" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="H7" s="9" t="str">
         <f>Spiece!$A$4</f>
         <v>003</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B8" s="10">
         <v>44873</v>
       </c>
       <c r="C8" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D8" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>30</v>
+        <v>227</v>
       </c>
       <c r="F8" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="H8" s="9" t="str">
         <f>Spiece!$A$5</f>
         <v>004</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B9" s="10">
         <v>44874</v>
       </c>
       <c r="C9" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>30</v>
+        <v>227</v>
       </c>
       <c r="F9" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="H9" s="9" t="str">
         <f>Spiece!$A$5</f>
         <v>004</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B10" s="10">
         <v>44875</v>
       </c>
       <c r="C10" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>9</v>
+        <v>224</v>
       </c>
       <c r="F10" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="H10" s="9" t="str">
         <f>Spiece!$A$2</f>
         <v>001</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B11" s="10">
         <v>44876</v>
       </c>
       <c r="C11" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>9</v>
+        <v>224</v>
       </c>
       <c r="F11" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="H11" s="9" t="str">
         <f>Spiece!$A$2</f>
         <v>001</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B12" s="10">
         <v>44877</v>
       </c>
       <c r="C12" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>18</v>
+        <v>225</v>
       </c>
       <c r="F12" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="H12" s="9" t="str">
         <f>Spiece!$A$3</f>
         <v>002</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B13" s="10">
         <v>44878</v>
       </c>
       <c r="C13" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>18</v>
+        <v>225</v>
       </c>
       <c r="F13" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="H13" s="9" t="str">
         <f>Spiece!$A$3</f>
         <v>002</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B14" s="10">
         <v>44879</v>
       </c>
       <c r="C14" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D14" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>18</v>
+        <v>225</v>
       </c>
       <c r="F14" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="H14" s="9" t="str">
         <f>Spiece!$A$3</f>
         <v>002</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B15" s="10">
         <v>44880</v>
       </c>
       <c r="C15" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>25</v>
+        <v>226</v>
       </c>
       <c r="F15" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="H15" s="9" t="str">
         <f>Spiece!$A$4</f>
         <v>003</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B16" s="10">
         <v>44881</v>
       </c>
       <c r="C16" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>30</v>
+        <v>227</v>
       </c>
       <c r="F16" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="H16" s="9" t="str">
         <f>Spiece!$A$5</f>
         <v>004</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B17" s="10">
         <v>44882</v>
       </c>
       <c r="C17" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>30</v>
+        <v>227</v>
       </c>
       <c r="F17" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="H17" s="9" t="str">
         <f>Spiece!$A$5</f>
         <v>004</v>
       </c>
       <c r="I17" s="9" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B18" s="10">
         <v>44883</v>
       </c>
       <c r="C18" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>18</v>
+        <v>225</v>
       </c>
       <c r="F18" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="H18" s="9" t="str">
         <f>Spiece!$A$3</f>
         <v>002</v>
       </c>
       <c r="I18" s="9" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B19" s="10">
         <v>44884</v>
       </c>
       <c r="C19" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>9</v>
+        <v>224</v>
       </c>
       <c r="F19" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="H19" s="9" t="str">
         <f>Spiece!$A$2</f>
         <v>001</v>
       </c>
       <c r="I19" s="9" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://upload.wikimedia.org/wikipedia/commons/thumb/f/fa/Red-whiskered_bulbul_by_Creepanta_11.jpg/420px-Red-whiskered_bulbul_by_Creepanta_11.jpg" xr:uid="{9D11F141-8192-4B78-8975-5545840D3054}"/>
-    <hyperlink ref="E3" r:id="rId2" display="https://upload.wikimedia.org/wikipedia/commons/thumb/f/fa/Red-whiskered_bulbul_by_Creepanta_11.jpg/420px-Red-whiskered_bulbul_by_Creepanta_11.jpg" xr:uid="{E772DBE9-6628-415E-9E57-0CFA5DF69C6B}"/>
-    <hyperlink ref="E10" r:id="rId3" display="https://upload.wikimedia.org/wikipedia/commons/thumb/f/fa/Red-whiskered_bulbul_by_Creepanta_11.jpg/420px-Red-whiskered_bulbul_by_Creepanta_11.jpg" xr:uid="{7E1B40F7-1ABE-4FA7-9EA9-9B344C169A93}"/>
-    <hyperlink ref="E11" r:id="rId4" display="https://upload.wikimedia.org/wikipedia/commons/thumb/f/fa/Red-whiskered_bulbul_by_Creepanta_11.jpg/420px-Red-whiskered_bulbul_by_Creepanta_11.jpg" xr:uid="{642D735D-2C03-43A2-860E-C7000686E829}"/>
-    <hyperlink ref="E19" r:id="rId5" display="https://upload.wikimedia.org/wikipedia/commons/thumb/f/fa/Red-whiskered_bulbul_by_Creepanta_11.jpg/420px-Red-whiskered_bulbul_by_Creepanta_11.jpg" xr:uid="{4A555574-FFF7-41FD-A258-B5FFADD2FADF}"/>
-    <hyperlink ref="E4" r:id="rId6" display="https://cdn.eva.vn/upload/3-2021/images/2021-09-30/image3-1632998835-30-width650height460.jpg" xr:uid="{9CDF5B10-F25E-40D0-88C0-FFBB102FF84A}"/>
-    <hyperlink ref="E5" r:id="rId7" display="https://cdn.eva.vn/upload/3-2021/images/2021-09-30/image3-1632998835-30-width650height460.jpg" xr:uid="{A833710E-826E-431B-834D-C6690DF095A2}"/>
-    <hyperlink ref="E18" r:id="rId8" display="https://cdn.eva.vn/upload/3-2021/images/2021-09-30/image3-1632998835-30-width650height460.jpg" xr:uid="{B5F2595A-5944-4D3E-B20D-29299A992251}"/>
-    <hyperlink ref="E12" r:id="rId9" display="https://cdn.eva.vn/upload/3-2021/images/2021-09-30/image3-1632998835-30-width650height460.jpg" xr:uid="{9BBFDD6B-BC8C-4310-B38F-BA0BB0CDC1CA}"/>
-    <hyperlink ref="E13" r:id="rId10" display="https://cdn.eva.vn/upload/3-2021/images/2021-09-30/image3-1632998835-30-width650height460.jpg" xr:uid="{40D41F0E-102E-46F5-A174-6DF0DCD621FC}"/>
-    <hyperlink ref="E14" r:id="rId11" display="https://cdn.eva.vn/upload/3-2021/images/2021-09-30/image3-1632998835-30-width650height460.jpg" xr:uid="{C97B23DA-72FD-4DD5-92DC-05B6EC37F93B}"/>
-    <hyperlink ref="E15" r:id="rId12" display="https://lh3.googleusercontent.com/x2qa9iwXtlPBwn3_s0Of700Z45jLsv3y_qHdrfsHTbEJbKGaQFlCIgMp7BsVeHNDY_t1Y3FZyTk44hwXnY9ZTymKEGOe8dMiBsEyM3X_jFZN11XQX2yw4OC_a8ef_8mlPk5jD0Gn" xr:uid="{46712425-A4F7-47B6-8A40-35149611F2F6}"/>
-    <hyperlink ref="E6" r:id="rId13" display="https://lh3.googleusercontent.com/x2qa9iwXtlPBwn3_s0Of700Z45jLsv3y_qHdrfsHTbEJbKGaQFlCIgMp7BsVeHNDY_t1Y3FZyTk44hwXnY9ZTymKEGOe8dMiBsEyM3X_jFZN11XQX2yw4OC_a8ef_8mlPk5jD0Gn" xr:uid="{E975EFD5-B2D8-4DC9-9514-6E3BC3FBA3A6}"/>
-    <hyperlink ref="E7" r:id="rId14" display="https://lh3.googleusercontent.com/x2qa9iwXtlPBwn3_s0Of700Z45jLsv3y_qHdrfsHTbEJbKGaQFlCIgMp7BsVeHNDY_t1Y3FZyTk44hwXnY9ZTymKEGOe8dMiBsEyM3X_jFZN11XQX2yw4OC_a8ef_8mlPk5jD0Gn" xr:uid="{D1E8D307-EC2C-4BBD-A30C-1872B460638C}"/>
-    <hyperlink ref="E16" r:id="rId15" display="https://cdn.eva.vn/upload/4-2021/images/2021-10-01/image1-1633053449-421-width600height450.jpg" xr:uid="{E2C522BF-8780-485D-954F-EBAA279BDC39}"/>
-    <hyperlink ref="E17" r:id="rId16" display="https://cdn.eva.vn/upload/4-2021/images/2021-10-01/image1-1633053449-421-width600height450.jpg" xr:uid="{AB74E273-4646-4D80-9332-1A1646832C30}"/>
-    <hyperlink ref="E9" r:id="rId17" display="https://cdn.eva.vn/upload/4-2021/images/2021-10-01/image1-1633053449-421-width600height450.jpg" xr:uid="{D74D690A-0B52-4327-807C-95599AB06E16}"/>
-    <hyperlink ref="E8" r:id="rId18" display="https://cdn.eva.vn/upload/4-2021/images/2021-10-01/image1-1633053449-421-width600height450.jpg" xr:uid="{6FC57DE8-2808-4E5F-889E-CCCAF2C8BC6C}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{DF8B9C05-0922-4B7A-B893-839536FAD19F}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{09DB027A-DCE4-44E6-BA4B-0E531C859224}"/>
+    <hyperlink ref="E10" r:id="rId3" xr:uid="{A2B71AF2-29E6-4FF4-93E8-18664CA422DF}"/>
+    <hyperlink ref="E11" r:id="rId4" xr:uid="{15485CE2-3E9A-49F3-91DD-CF90EE939A0D}"/>
+    <hyperlink ref="E19" r:id="rId5" xr:uid="{B77E4E0E-ED1D-4329-87CB-ED323039714E}"/>
+    <hyperlink ref="E12" r:id="rId6" xr:uid="{1090702A-4317-44BE-9631-65EC5F59C4D9}"/>
+    <hyperlink ref="E13" r:id="rId7" xr:uid="{9E353F11-5D07-429A-8ABE-6C8B9F4F5B24}"/>
+    <hyperlink ref="E14" r:id="rId8" xr:uid="{1134FA98-1308-44E4-A31B-5A05951AD2A4}"/>
+    <hyperlink ref="E18" r:id="rId9" xr:uid="{C1E21B79-47D8-469E-95C8-A048465AC549}"/>
+    <hyperlink ref="E4" r:id="rId10" xr:uid="{7A1042E7-EEBA-4EA0-8172-B859027A890D}"/>
+    <hyperlink ref="E5" r:id="rId11" xr:uid="{9A6F4DCB-B8C5-4865-B531-EF9B28B01333}"/>
+    <hyperlink ref="E6" r:id="rId12" xr:uid="{FB4E98F1-E6D1-4BFA-A075-8038902423EF}"/>
+    <hyperlink ref="E7" r:id="rId13" xr:uid="{6740460D-C8EA-4BA2-86B7-D4FCC08792A3}"/>
+    <hyperlink ref="E15" r:id="rId14" xr:uid="{35992581-E13D-46B2-B60F-7D4FB472834B}"/>
+    <hyperlink ref="E8" r:id="rId15" xr:uid="{B5FEBA26-B8A7-4BEC-A046-BC75C90441E0}"/>
+    <hyperlink ref="E9" r:id="rId16" xr:uid="{8CD88F44-1592-4D12-B514-A71A5B617161}"/>
+    <hyperlink ref="E16" r:id="rId17" xr:uid="{9E3EDD69-5A4C-437E-8BB2-060422839466}"/>
+    <hyperlink ref="E17" r:id="rId18" xr:uid="{32229944-11E8-4315-B644-5C15A4E19008}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1825,10 +1855,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA9E6B09-073D-4E09-9856-D8ACA7A9A17A}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1849,36 +1879,36 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D2" t="s">
         <v>94</v>
       </c>
-      <c r="C2" t="s">
-        <v>101</v>
-      </c>
-      <c r="D2" t="s">
-        <v>98</v>
-      </c>
       <c r="E2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="F2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="G2">
         <v>2</v>
@@ -1886,22 +1916,22 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B3" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C3" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E3" t="s">
         <v>107</v>
       </c>
-      <c r="E3" t="s">
-        <v>111</v>
-      </c>
       <c r="F3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="G3">
         <v>2</v>
@@ -1909,22 +1939,22 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B4" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D4" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E4" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F4" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="G4">
         <v>20</v>
@@ -1932,22 +1962,22 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B5" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C5" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D5" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E5" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F5" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="G5">
         <v>20</v>
@@ -1955,22 +1985,22 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B6" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C6" t="s">
+        <v>99</v>
+      </c>
+      <c r="D6" t="s">
         <v>103</v>
       </c>
-      <c r="D6" t="s">
-        <v>107</v>
-      </c>
       <c r="E6" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F6" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="G6">
         <v>2</v>
@@ -1978,22 +2008,22 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B7" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C7" t="s">
+        <v>99</v>
+      </c>
+      <c r="D7" t="s">
         <v>103</v>
       </c>
-      <c r="D7" t="s">
-        <v>107</v>
-      </c>
       <c r="E7" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F7" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="G7">
         <v>2</v>
@@ -2001,22 +2031,22 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B8" t="s">
+        <v>106</v>
+      </c>
+      <c r="C8" t="s">
+        <v>97</v>
+      </c>
+      <c r="D8" t="s">
+        <v>103</v>
+      </c>
+      <c r="E8" t="s">
         <v>110</v>
       </c>
-      <c r="C8" t="s">
-        <v>101</v>
-      </c>
-      <c r="D8" t="s">
-        <v>107</v>
-      </c>
-      <c r="E8" t="s">
-        <v>114</v>
-      </c>
       <c r="F8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="G8">
         <v>5</v>
@@ -2024,22 +2054,22 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B9" t="s">
         <v>92</v>
       </c>
-      <c r="B9" t="s">
-        <v>96</v>
-      </c>
       <c r="C9" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D9" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E9" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F9" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="G9">
         <v>2</v>
@@ -2047,22 +2077,22 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B10" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C10" t="s">
+        <v>105</v>
+      </c>
+      <c r="D10" t="s">
+        <v>101</v>
+      </c>
+      <c r="E10" t="s">
         <v>109</v>
       </c>
-      <c r="D10" t="s">
-        <v>105</v>
-      </c>
-      <c r="E10" t="s">
-        <v>113</v>
-      </c>
       <c r="F10" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="G10">
         <v>1</v>
@@ -2070,25 +2100,48 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B11" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C11" t="s">
+        <v>105</v>
+      </c>
+      <c r="D11" t="s">
+        <v>101</v>
+      </c>
+      <c r="E11" t="s">
         <v>109</v>
       </c>
-      <c r="D11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E11" t="s">
-        <v>113</v>
-      </c>
       <c r="F11" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="G11">
         <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="B12" t="s">
+        <v>93</v>
+      </c>
+      <c r="C12" t="s">
+        <v>95</v>
+      </c>
+      <c r="D12" t="s">
+        <v>100</v>
+      </c>
+      <c r="E12" t="s">
+        <v>108</v>
+      </c>
+      <c r="F12" t="s">
+        <v>68</v>
+      </c>
+      <c r="G12">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -2099,12 +2152,643 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63A21F89-FFB6-4442-99E8-81576EE85D5E}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B19" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41:E42"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="8.88671875" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" customWidth="1"/>
+    <col min="5" max="5" width="27.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C1" t="s">
+        <v>230</v>
+      </c>
+      <c r="D1" t="s">
+        <v>231</v>
+      </c>
+      <c r="E1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="D2" s="10">
+        <v>44867</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="D3" s="10">
+        <v>44868</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="D4" s="10">
+        <v>44869</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="D5" s="10">
+        <v>44870</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="D6" s="10">
+        <v>44871</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="D7" s="10">
+        <v>44872</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="D8" s="10">
+        <v>44873</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="D9" s="10">
+        <v>44874</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="D10" s="10">
+        <v>44875</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="D11" s="10">
+        <v>44876</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="D12" s="10">
+        <v>44877</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="D13" s="10">
+        <v>44878</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="D14" s="10">
+        <v>44879</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="D15" s="10">
+        <v>44879</v>
+      </c>
+      <c r="E15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="D16" s="10">
+        <v>44880</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="D17" s="10">
+        <v>44881</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="D18" s="10">
+        <v>44882</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="D19" s="10">
+        <v>44883</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="D20" s="10">
+        <v>44884</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B21" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D21" s="10">
+        <v>44931</v>
+      </c>
+      <c r="E21" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B22" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D22" s="10">
+        <v>44931</v>
+      </c>
+      <c r="E22" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B23" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D23" s="10">
+        <v>44931</v>
+      </c>
+      <c r="E23" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B24" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D24" s="10">
+        <v>44931</v>
+      </c>
+      <c r="E24" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B25" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D25" s="10">
+        <v>44931</v>
+      </c>
+      <c r="E25" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B26" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D26" s="10">
+        <v>44931</v>
+      </c>
+      <c r="E26" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B27" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D27" s="10">
+        <v>44931</v>
+      </c>
+      <c r="E27" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B28" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D28" s="10">
+        <v>44931</v>
+      </c>
+      <c r="E28" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B29" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D29" s="10">
+        <v>44931</v>
+      </c>
+      <c r="E29" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B30" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D30" s="10">
+        <v>44931</v>
+      </c>
+      <c r="E30" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B31" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D31" s="10">
+        <v>44931</v>
+      </c>
+      <c r="E31" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B32" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D32" s="10">
+        <v>44931</v>
+      </c>
+      <c r="E32" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B33" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D33" s="10">
+        <v>44931</v>
+      </c>
+      <c r="E33" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B34" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D34" s="10">
+        <v>44931</v>
+      </c>
+      <c r="E34" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B35" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D35" s="10">
+        <v>44931</v>
+      </c>
+      <c r="E35" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B36" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D36" s="10">
+        <v>44931</v>
+      </c>
+      <c r="E36" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B37" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D37" s="10">
+        <v>44931</v>
+      </c>
+      <c r="E37" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B38" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="D38" s="10">
+        <v>45225</v>
+      </c>
+      <c r="E38" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B39" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="D39" s="10">
+        <v>45225</v>
+      </c>
+      <c r="E39" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B40" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="D40" s="10">
+        <v>45230</v>
+      </c>
+      <c r="E40" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B41" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D41" s="10">
+        <v>45230</v>
+      </c>
+      <c r="E41" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B42" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D42" s="10">
+        <v>45230</v>
+      </c>
+      <c r="E42" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B43" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D43" s="10">
+        <v>45231</v>
+      </c>
+      <c r="E43" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B44" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D44" s="10">
+        <v>45231</v>
+      </c>
+      <c r="E44" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2113,7 +2797,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AED08018-F18A-4DAC-B772-EE2F04BE56C9}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
@@ -2131,265 +2815,265 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D1" t="s">
+        <v>200</v>
+      </c>
+      <c r="E1" t="s">
+        <v>201</v>
+      </c>
+      <c r="F1" t="s">
         <v>202</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" t="s">
         <v>203</v>
-      </c>
-      <c r="D1" t="s">
-        <v>204</v>
-      </c>
-      <c r="E1" t="s">
-        <v>205</v>
-      </c>
-      <c r="F1" t="s">
-        <v>206</v>
-      </c>
-      <c r="G1" t="s">
-        <v>38</v>
-      </c>
-      <c r="H1" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="B2" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="E2" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B3" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="D3" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="E3" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="B4" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="E4" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="B5" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="E5" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="B6" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="E6" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B7" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="E7" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="B8" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="E8" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="B9" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="E9" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="B10" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E10" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="B11" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E11" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="B12" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E12" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B13" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E13" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -2418,263 +3102,263 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C1" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="D1" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="E1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="F1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="E2" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="E3" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="E4" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="F4" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="E5" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="F5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="E6" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="E7" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="E8" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="E9" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="E10" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="E11" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E12" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E13" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E14" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E15" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -2709,155 +3393,155 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D1" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="G1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="H1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D2">
         <v>60</v>
       </c>
       <c r="E2" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="F2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D3">
         <v>60</v>
       </c>
       <c r="E3" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="F3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D4">
         <v>30</v>
       </c>
       <c r="E4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F4" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="G4" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D5">
         <v>31</v>
       </c>
       <c r="E5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F5" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="G5" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D6">
         <v>32</v>
       </c>
       <c r="E6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F6" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="G6" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -2878,27 +3562,27 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D2">
         <v>0.01</v>
@@ -2906,13 +3590,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D3">
         <v>5.0000000000000001E-3</v>
@@ -2920,13 +3604,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D4">
         <v>6.3E-2</v>
@@ -2934,13 +3618,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D5">
         <v>0.05</v>
@@ -2948,13 +3632,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D6">
         <v>0.01</v>
@@ -2962,13 +3646,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D7">
         <v>0.08</v>
@@ -2976,13 +3660,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D8">
         <v>5.0000000000000001E-3</v>
@@ -2990,13 +3674,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D9">
         <v>3.5000000000000003E-2</v>
@@ -3004,13 +3688,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D10">
         <v>0.01</v>
@@ -3018,13 +3702,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D11">
         <v>0.08</v>
@@ -3032,13 +3716,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -3046,13 +3730,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D13">
         <v>0.01</v>
@@ -3060,13 +3744,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D14">
         <v>0.08</v>
@@ -3074,13 +3758,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -3111,45 +3795,45 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="D1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="F1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="G1" t="s">
         <v>7</v>
       </c>
       <c r="H1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E2" t="s">
         <v>141</v>
-      </c>
-      <c r="D2" t="s">
-        <v>143</v>
-      </c>
-      <c r="E2" t="s">
-        <v>145</v>
       </c>
       <c r="F2">
         <v>250000</v>
@@ -3163,19 +3847,19 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C3" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D3" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E3" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F3">
         <v>350000</v>
@@ -3189,19 +3873,19 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B4" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D4" t="s">
         <v>139</v>
       </c>
-      <c r="D4" t="s">
-        <v>143</v>
-      </c>
       <c r="E4" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F4">
         <v>70000</v>
@@ -3215,19 +3899,19 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B5" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C5" t="s">
+        <v>136</v>
+      </c>
+      <c r="D5" t="s">
         <v>140</v>
       </c>
-      <c r="D5" t="s">
-        <v>144</v>
-      </c>
       <c r="E5" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F5">
         <v>30000</v>
@@ -3241,19 +3925,19 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B6" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D6" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="E6" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F6">
         <v>25000</v>
@@ -3267,16 +3951,16 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B7" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D7" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E7" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F7">
         <v>15000</v>
@@ -3290,16 +3974,16 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B8" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D8" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="E8" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F8">
         <v>45000</v>
@@ -3313,19 +3997,19 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B9" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D9" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E9" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F9">
         <v>40000</v>
@@ -3339,19 +4023,19 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B10" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D10" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E10" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F10">
         <v>32000</v>
@@ -3365,16 +4049,16 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B11" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D11" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E11" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F11">
         <v>100000</v>
@@ -3388,16 +4072,16 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B12" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D12" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E12" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F12">
         <v>50000</v>
@@ -3411,16 +4095,16 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="B13" t="s">
+        <v>176</v>
+      </c>
+      <c r="D13" t="s">
         <v>177</v>
       </c>
-      <c r="B13" t="s">
-        <v>180</v>
-      </c>
-      <c r="D13" t="s">
-        <v>181</v>
-      </c>
       <c r="E13" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="F13">
         <v>120000</v>
@@ -3434,16 +4118,16 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="B14" t="s">
+        <v>169</v>
+      </c>
+      <c r="D14" t="s">
+        <v>177</v>
+      </c>
+      <c r="E14" t="s">
         <v>178</v>
-      </c>
-      <c r="B14" t="s">
-        <v>173</v>
-      </c>
-      <c r="D14" t="s">
-        <v>181</v>
-      </c>
-      <c r="E14" t="s">
-        <v>182</v>
       </c>
       <c r="F14">
         <v>150000</v>
@@ -3457,16 +4141,16 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B15" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D15" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E15" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F15">
         <v>120000</v>

</xml_diff>